<commit_message>
beto telas e procs
</commit_message>
<xml_diff>
--- a/Planejamento/Tarefas.xlsx
+++ b/Planejamento/Tarefas.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Romulo\Documents\GitHub\InfoTech2u\Planejamento\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Home\Documents\GitHub\InfoTech2u\Planejamento\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -17,7 +17,7 @@
   </sheets>
   <calcPr calcId="152511"/>
   <pivotCaches>
-    <pivotCache cacheId="11" r:id="rId3"/>
+    <pivotCache cacheId="0" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -163,7 +163,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -171,13 +171,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="10">
@@ -303,7 +315,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -319,29 +331,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="10">
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
@@ -478,6 +475,22 @@
       </border>
     </dxf>
     <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <border>
         <bottom style="thin">
           <color indexed="64"/>
@@ -492,12 +505,14 @@
         <right style="thin">
           <color indexed="64"/>
         </right>
-        <top style="thin">
+        <top/>
+        <bottom/>
+        <vertical style="thin">
           <color indexed="64"/>
-        </top>
-        <bottom style="thin">
+        </vertical>
+        <horizontal style="thin">
           <color indexed="64"/>
-        </bottom>
+        </horizontal>
       </border>
     </dxf>
   </dxfs>
@@ -532,7 +547,6 @@
   </c:pivotSource>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -611,49 +625,7 @@
           </a:effectLst>
         </c:spPr>
         <c:marker>
-          <c:symbol val="circle"/>
-          <c:size val="6"/>
-          <c:spPr>
-            <a:gradFill rotWithShape="1">
-              <a:gsLst>
-                <a:gs pos="0">
-                  <a:schemeClr val="accent1">
-                    <a:satMod val="103000"/>
-                    <a:lumMod val="102000"/>
-                    <a:tint val="94000"/>
-                  </a:schemeClr>
-                </a:gs>
-                <a:gs pos="50000">
-                  <a:schemeClr val="accent1">
-                    <a:satMod val="110000"/>
-                    <a:lumMod val="100000"/>
-                    <a:shade val="100000"/>
-                  </a:schemeClr>
-                </a:gs>
-                <a:gs pos="100000">
-                  <a:schemeClr val="accent1">
-                    <a:lumMod val="99000"/>
-                    <a:satMod val="120000"/>
-                    <a:shade val="78000"/>
-                  </a:schemeClr>
-                </a:gs>
-              </a:gsLst>
-              <a:lin ang="5400000" scaled="0"/>
-            </a:gradFill>
-            <a:ln w="9525">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst>
-              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-                <a:srgbClr val="000000">
-                  <a:alpha val="63000"/>
-                </a:srgbClr>
-              </a:outerShdw>
-            </a:effectLst>
-          </c:spPr>
+          <c:symbol val="none"/>
         </c:marker>
       </c:pivotFmt>
     </c:pivotFmts>
@@ -816,11 +788,11 @@
         </c:dLbls>
         <c:gapWidth val="100"/>
         <c:overlap val="-24"/>
-        <c:axId val="614508944"/>
-        <c:axId val="613926400"/>
+        <c:axId val="545161088"/>
+        <c:axId val="545161632"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="614508944"/>
+        <c:axId val="545161088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -862,7 +834,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="613926400"/>
+        <c:crossAx val="545161632"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -870,7 +842,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="613926400"/>
+        <c:axId val="545161632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -920,7 +892,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="614508944"/>
+        <c:crossAx val="545161088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -934,7 +906,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1041,7 +1012,6 @@
   </c:pivotSource>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1105,12 +1075,10 @@
           </a:effectLst>
         </c:spPr>
         <c:marker>
-          <c:symbol val="circle"/>
-          <c:size val="6"/>
+          <c:symbol val="none"/>
         </c:marker>
         <c:dLbl>
           <c:idx val="0"/>
-          <c:layout/>
           <c:spPr>
             <a:noFill/>
             <a:ln>
@@ -1145,11 +1113,121 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
           <c:extLst>
-            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-              <c15:layout/>
-            </c:ext>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
           </c:extLst>
         </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="2"/>
+        <c:spPr>
+          <a:gradFill>
+            <a:gsLst>
+              <a:gs pos="0">
+                <a:schemeClr val="accent1"/>
+              </a:gs>
+              <a:gs pos="100000">
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="84000"/>
+                </a:schemeClr>
+              </a:gs>
+            </a:gsLst>
+            <a:lin ang="5400000" scaled="1"/>
+          </a:gradFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst>
+            <a:outerShdw blurRad="76200" dir="18900000" sy="23000" kx="-1200000" algn="bl" rotWithShape="0">
+              <a:prstClr val="black">
+                <a:alpha val="20000"/>
+              </a:prstClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="3"/>
+        <c:spPr>
+          <a:gradFill>
+            <a:gsLst>
+              <a:gs pos="0">
+                <a:schemeClr val="accent1"/>
+              </a:gs>
+              <a:gs pos="100000">
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="84000"/>
+                </a:schemeClr>
+              </a:gs>
+            </a:gsLst>
+            <a:lin ang="5400000" scaled="1"/>
+          </a:gradFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst>
+            <a:outerShdw blurRad="76200" dir="18900000" sy="23000" kx="-1200000" algn="bl" rotWithShape="0">
+              <a:prstClr val="black">
+                <a:alpha val="20000"/>
+              </a:prstClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="4"/>
+        <c:spPr>
+          <a:gradFill>
+            <a:gsLst>
+              <a:gs pos="0">
+                <a:schemeClr val="accent1"/>
+              </a:gs>
+              <a:gs pos="100000">
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="84000"/>
+                </a:schemeClr>
+              </a:gs>
+            </a:gsLst>
+            <a:lin ang="5400000" scaled="1"/>
+          </a:gradFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst>
+            <a:outerShdw blurRad="76200" dir="18900000" sy="23000" kx="-1200000" algn="bl" rotWithShape="0">
+              <a:prstClr val="black">
+                <a:alpha val="20000"/>
+              </a:prstClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="5"/>
+        <c:spPr>
+          <a:gradFill>
+            <a:gsLst>
+              <a:gs pos="0">
+                <a:schemeClr val="accent1"/>
+              </a:gs>
+              <a:gs pos="100000">
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="84000"/>
+                </a:schemeClr>
+              </a:gs>
+            </a:gsLst>
+            <a:lin ang="5400000" scaled="1"/>
+          </a:gradFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst>
+            <a:outerShdw blurRad="76200" dir="18900000" sy="23000" kx="-1200000" algn="bl" rotWithShape="0">
+              <a:prstClr val="black">
+                <a:alpha val="20000"/>
+              </a:prstClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </c:spPr>
       </c:pivotFmt>
     </c:pivotFmts>
     <c:plotArea>
@@ -1335,9 +1413,7 @@
               </c:spPr>
             </c:leaderLines>
             <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
-              </c:ext>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
             </c:extLst>
           </c:dLbls>
           <c:cat>
@@ -1403,7 +1479,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1514,7 +1589,6 @@
   </c:pivotSource>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1554,6 +1628,91 @@
     <c:pivotFmts>
       <c:pivotFmt>
         <c:idx val="0"/>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="1"/>
+        <c:spPr>
+          <a:gradFill rotWithShape="1">
+            <a:gsLst>
+              <a:gs pos="0">
+                <a:schemeClr val="accent1">
+                  <a:satMod val="103000"/>
+                  <a:lumMod val="102000"/>
+                  <a:tint val="94000"/>
+                </a:schemeClr>
+              </a:gs>
+              <a:gs pos="50000">
+                <a:schemeClr val="accent1">
+                  <a:satMod val="110000"/>
+                  <a:lumMod val="100000"/>
+                  <a:shade val="100000"/>
+                </a:schemeClr>
+              </a:gs>
+              <a:gs pos="100000">
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="99000"/>
+                  <a:satMod val="120000"/>
+                  <a:shade val="78000"/>
+                </a:schemeClr>
+              </a:gs>
+            </a:gsLst>
+            <a:lin ang="5400000" scaled="0"/>
+          </a:gradFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="2"/>
+        <c:spPr>
+          <a:gradFill rotWithShape="1">
+            <a:gsLst>
+              <a:gs pos="0">
+                <a:schemeClr val="accent1">
+                  <a:satMod val="103000"/>
+                  <a:lumMod val="102000"/>
+                  <a:tint val="94000"/>
+                </a:schemeClr>
+              </a:gs>
+              <a:gs pos="50000">
+                <a:schemeClr val="accent1">
+                  <a:satMod val="110000"/>
+                  <a:lumMod val="100000"/>
+                  <a:shade val="100000"/>
+                </a:schemeClr>
+              </a:gs>
+              <a:gs pos="100000">
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="99000"/>
+                  <a:satMod val="120000"/>
+                  <a:shade val="78000"/>
+                </a:schemeClr>
+              </a:gs>
+            </a:gsLst>
+            <a:lin ang="5400000" scaled="0"/>
+          </a:gradFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </c:spPr>
       </c:pivotFmt>
     </c:pivotFmts>
     <c:plotArea>
@@ -1661,7 +1820,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3895,126 +4053,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tabela dinâmica3" cacheId="11" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="5">
-  <location ref="A35:B37" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="6">
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisRow" dataField="1" showAll="0">
-      <items count="3">
-        <item m="1" x="1"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="5"/>
-  </rowFields>
-  <rowItems count="2">
-    <i>
-      <x v="1"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Contagem de Status" fld="5" subtotal="count" baseField="0" baseItem="0"/>
-  </dataFields>
-  <chartFormats count="1">
-    <chartFormat chart="0" format="1" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-  </chartFormats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tabela dinâmica2" cacheId="11" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="7">
-  <location ref="A19:B24" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="6">
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="5">
-        <item x="2"/>
-        <item x="0"/>
-        <item x="1"/>
-        <item x="3"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="4"/>
-  </rowFields>
-  <rowItems count="5">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Contagem de Pagina" fld="3" subtotal="count" baseField="0" baseItem="0"/>
-  </dataFields>
-  <chartFormats count="1">
-    <chartFormat chart="0" format="1" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-  </chartFormats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tabela dinâmica1" cacheId="11" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tabela dinâmica1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3">
   <location ref="A1:B14" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="6">
     <pivotField showAll="0"/>
@@ -4110,19 +4149,197 @@
 </pivotTableDefinition>
 </file>
 
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tabela dinâmica3" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="5">
+  <location ref="A35:B37" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="6">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" dataField="1" showAll="0">
+      <items count="3">
+        <item m="1" x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="5"/>
+  </rowFields>
+  <rowItems count="2">
+    <i>
+      <x v="1"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Contagem de Status" fld="5" subtotal="count" baseField="0" baseItem="0"/>
+  </dataFields>
+  <chartFormats count="2">
+    <chartFormat chart="0" format="1" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="2">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="5" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tabela dinâmica2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="7">
+  <location ref="A19:B24" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="6">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="5">
+        <item x="2"/>
+        <item x="0"/>
+        <item x="1"/>
+        <item x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="4"/>
+  </rowFields>
+  <rowItems count="5">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Contagem de Pagina" fld="3" subtotal="count" baseField="0" baseItem="0"/>
+  </dataFields>
+  <chartFormats count="5">
+    <chartFormat chart="0" format="1" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="2">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="4" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="3">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="4" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="4">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="4" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="5">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="4" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:F40" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="8" tableBorderDxfId="9" totalsRowBorderDxfId="7">
-  <autoFilter ref="A1:F40"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:F40" totalsRowShown="0" headerRowDxfId="9" headerRowBorderDxfId="8" tableBorderDxfId="7" totalsRowBorderDxfId="6">
   <sortState ref="A2:D13">
     <sortCondition ref="A1:A13"/>
   </sortState>
   <tableColumns count="6">
-    <tableColumn id="1" name="Prioridade" dataDxfId="6"/>
-    <tableColumn id="2" name="Agrupamento" dataDxfId="5"/>
-    <tableColumn id="3" name="Funcionalidade" dataDxfId="4"/>
-    <tableColumn id="4" name="Pagina" dataDxfId="3"/>
-    <tableColumn id="5" name="Responsavel" dataDxfId="2"/>
-    <tableColumn id="6" name="Status" dataDxfId="1"/>
+    <tableColumn id="1" name="Prioridade" dataDxfId="5"/>
+    <tableColumn id="2" name="Agrupamento" dataDxfId="4"/>
+    <tableColumn id="3" name="Funcionalidade" dataDxfId="3"/>
+    <tableColumn id="4" name="Pagina" dataDxfId="2"/>
+    <tableColumn id="5" name="Responsavel" dataDxfId="1"/>
+    <tableColumn id="6" name="Status" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4393,8 +4610,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4588,242 +4805,242 @@
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="7">
+      <c r="A10" s="13">
         <v>3</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="C10" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="D10" s="8" t="s">
+      <c r="D10" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="E10" s="8" t="s">
+      <c r="E10" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="F10" s="9" t="s">
+      <c r="F10" s="15" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="7">
+      <c r="A11" s="13">
         <v>4</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="C11" s="8" t="s">
+      <c r="C11" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="D11" s="8" t="s">
+      <c r="D11" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="E11" s="8" t="s">
+      <c r="E11" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="F11" s="9" t="s">
+      <c r="F11" s="15" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="7">
+      <c r="A12" s="13">
         <v>4</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="B12" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="C12" s="8" t="s">
+      <c r="C12" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="D12" s="8" t="s">
+      <c r="D12" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="E12" s="8" t="s">
+      <c r="E12" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="F12" s="9" t="s">
+      <c r="F12" s="15" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="7">
+      <c r="A13" s="13">
         <v>4</v>
       </c>
-      <c r="B13" s="8" t="s">
+      <c r="B13" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="C13" s="8" t="s">
+      <c r="C13" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="D13" s="8" t="s">
+      <c r="D13" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="E13" s="8" t="s">
+      <c r="E13" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="F13" s="9" t="s">
+      <c r="F13" s="15" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="7">
+      <c r="A14" s="13">
         <v>4</v>
       </c>
-      <c r="B14" s="8" t="s">
+      <c r="B14" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="C14" s="8" t="s">
+      <c r="C14" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="D14" s="8" t="s">
+      <c r="D14" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="E14" s="8" t="s">
+      <c r="E14" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="F14" s="9" t="s">
+      <c r="F14" s="15" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="7">
+      <c r="A15" s="13">
         <v>4</v>
       </c>
-      <c r="B15" s="8" t="s">
+      <c r="B15" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="C15" s="8" t="s">
+      <c r="C15" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="D15" s="8" t="s">
+      <c r="D15" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="E15" s="8" t="s">
+      <c r="E15" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="F15" s="9" t="s">
+      <c r="F15" s="15" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="7">
+      <c r="A16" s="13">
         <v>4</v>
       </c>
-      <c r="B16" s="8" t="s">
+      <c r="B16" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="C16" s="8" t="s">
+      <c r="C16" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="D16" s="8" t="s">
+      <c r="D16" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="E16" s="8" t="s">
+      <c r="E16" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="F16" s="9" t="s">
+      <c r="F16" s="15" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="7">
+      <c r="A17" s="13">
         <v>4</v>
       </c>
-      <c r="B17" s="8" t="s">
+      <c r="B17" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="C17" s="8" t="s">
+      <c r="C17" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="D17" s="8" t="s">
+      <c r="D17" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="E17" s="8" t="s">
+      <c r="E17" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="F17" s="9" t="s">
+      <c r="F17" s="15" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="7">
+      <c r="A18" s="13">
         <v>4</v>
       </c>
-      <c r="B18" s="8" t="s">
+      <c r="B18" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="C18" s="8" t="s">
+      <c r="C18" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="D18" s="8" t="s">
+      <c r="D18" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="E18" s="8" t="s">
+      <c r="E18" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="F18" s="9" t="s">
+      <c r="F18" s="15" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="7">
+      <c r="A19" s="13">
         <v>4</v>
       </c>
-      <c r="B19" s="8" t="s">
+      <c r="B19" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="C19" s="8" t="s">
+      <c r="C19" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="D19" s="8" t="s">
+      <c r="D19" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="E19" s="8" t="s">
+      <c r="E19" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="F19" s="9" t="s">
+      <c r="F19" s="15" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="7">
+      <c r="A20" s="13">
         <v>4</v>
       </c>
-      <c r="B20" s="8" t="s">
+      <c r="B20" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="C20" s="8" t="s">
+      <c r="C20" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="D20" s="8" t="s">
+      <c r="D20" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="E20" s="8" t="s">
+      <c r="E20" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="F20" s="9" t="s">
+      <c r="F20" s="15" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="7">
+      <c r="A21" s="13">
         <v>4</v>
       </c>
-      <c r="B21" s="8" t="s">
+      <c r="B21" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="C21" s="8" t="s">
+      <c r="C21" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="D21" s="8" t="s">
+      <c r="D21" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="E21" s="8" t="s">
+      <c r="E21" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="F21" s="9" t="s">
+      <c r="F21" s="15" t="s">
         <v>40</v>
       </c>
     </row>
@@ -5209,8 +5426,9 @@
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>